<commit_message>
naprawiony problem z ładowaniem ścieżki do plików
</commit_message>
<xml_diff>
--- a/zlecenie 12.xlsx
+++ b/zlecenie 12.xlsx
@@ -2,10 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="Arkusz1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
@@ -26,6 +28,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -271,6 +274,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -286,8 +290,8 @@
       <c r="C1" s="1">
         <v>10.0</v>
       </c>
-      <c r="D1" s="1">
-        <v>0.0</v>
+      <c r="D1" s="1" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="2">
@@ -300,8 +304,8 @@
       <c r="C2" s="1">
         <v>20.0</v>
       </c>
-      <c r="D2" s="1">
-        <v>0.0</v>
+      <c r="D2" s="1" t="n">
+        <v>20.0</v>
       </c>
     </row>
     <row r="3">
@@ -314,8 +318,8 @@
       <c r="C3" s="1">
         <v>30.0</v>
       </c>
-      <c r="D3" s="1">
-        <v>0.0</v>
+      <c r="D3" s="1" t="n">
+        <v>30.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>